<commit_message>
[update] LeNet9 for CIFAR10 and VGG10 for MNIST
</commit_message>
<xml_diff>
--- a/results/LeNet5/LeNet5 results.xlsx
+++ b/results/LeNet5/LeNet5 results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MyCourse(5 delayed 1)\erasure code\SUSTech-Coded-Computation\results\LeNet5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EF79C3-7E0E-4BA3-B414-172CC8FC9144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F36902-6543-41BD-94CF-1C25CAEFC57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="6828" yWindow="312" windowWidth="10296" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -155,7 +155,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,12 +171,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -260,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -305,12 +299,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -595,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="M95" sqref="M95"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1749,21 +1737,21 @@
         <v>0.91300000000000003</v>
       </c>
       <c r="F39" s="11"/>
-      <c r="G39" s="16">
-        <v>1</v>
-      </c>
-      <c r="H39" s="17">
+      <c r="G39" s="14">
+        <v>1</v>
+      </c>
+      <c r="H39" s="15">
         <v>0.82509999999999994</v>
       </c>
-      <c r="I39" s="17">
+      <c r="I39" s="15">
         <f>D38-H39</f>
         <v>9.650000000000003E-2</v>
       </c>
-      <c r="J39" s="17">
+      <c r="J39" s="15">
         <f>H39/D39</f>
         <v>0.89529079861111105</v>
       </c>
-      <c r="K39" s="17">
+      <c r="K39" s="15">
         <f>H39/E39</f>
         <v>0.90372398685651689</v>
       </c>
@@ -1779,21 +1767,21 @@
         <v>0.91300000000000003</v>
       </c>
       <c r="F40" s="11"/>
-      <c r="G40" s="16">
+      <c r="G40" s="14">
         <v>2</v>
       </c>
-      <c r="H40" s="17">
+      <c r="H40" s="15">
         <v>0.70379999999999998</v>
       </c>
-      <c r="I40" s="17">
+      <c r="I40" s="15">
         <f>D38-H40</f>
         <v>0.21779999999999999</v>
       </c>
-      <c r="J40" s="17">
+      <c r="J40" s="15">
         <f>H40/D40</f>
         <v>0.763671875</v>
       </c>
-      <c r="K40" s="17">
+      <c r="K40" s="15">
         <f>H40/E40</f>
         <v>0.77086527929901416</v>
       </c>
@@ -2217,16 +2205,16 @@
       </c>
       <c r="E56" s="13"/>
       <c r="F56" s="6"/>
-      <c r="G56" s="16">
-        <v>1</v>
-      </c>
-      <c r="H56" s="17"/>
-      <c r="I56" s="17">
+      <c r="G56" s="14">
+        <v>1</v>
+      </c>
+      <c r="H56" s="15"/>
+      <c r="I56" s="15">
         <f>D56-H56</f>
         <v>0.99360000000000004</v>
       </c>
-      <c r="J56" s="17"/>
-      <c r="K56" s="17"/>
+      <c r="J56" s="15"/>
+      <c r="K56" s="15"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
@@ -2422,16 +2410,16 @@
       </c>
       <c r="E65" s="5"/>
       <c r="F65" s="11"/>
-      <c r="G65" s="16">
-        <v>1</v>
-      </c>
-      <c r="H65" s="17"/>
-      <c r="I65" s="17">
+      <c r="G65" s="14">
+        <v>1</v>
+      </c>
+      <c r="H65" s="15"/>
+      <c r="I65" s="15">
         <f t="shared" ref="I65:I77" si="11">D65-H65</f>
         <v>0.99360000000000004</v>
       </c>
-      <c r="J65" s="16"/>
-      <c r="K65" s="16"/>
+      <c r="J65" s="14"/>
+      <c r="K65" s="14"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="11"/>
@@ -2442,16 +2430,16 @@
       </c>
       <c r="E66" s="5"/>
       <c r="F66" s="11"/>
-      <c r="G66" s="16">
+      <c r="G66" s="14">
         <v>2</v>
       </c>
-      <c r="H66" s="17"/>
-      <c r="I66" s="17">
+      <c r="H66" s="15"/>
+      <c r="I66" s="15">
         <f t="shared" si="11"/>
         <v>0.99360000000000004</v>
       </c>
-      <c r="J66" s="16"/>
-      <c r="K66" s="16"/>
+      <c r="J66" s="14"/>
+      <c r="K66" s="14"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="11"/>
@@ -2762,16 +2750,16 @@
       </c>
       <c r="E82" s="13"/>
       <c r="F82" s="6"/>
-      <c r="G82" s="16">
-        <v>1</v>
-      </c>
-      <c r="H82" s="17"/>
-      <c r="I82" s="17">
+      <c r="G82" s="14">
+        <v>1</v>
+      </c>
+      <c r="H82" s="15"/>
+      <c r="I82" s="15">
         <f t="shared" ref="I82:I88" si="12">D82-H82</f>
         <v>0.92159999999999997</v>
       </c>
-      <c r="J82" s="17"/>
-      <c r="K82" s="17"/>
+      <c r="J82" s="15"/>
+      <c r="K82" s="15"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>
@@ -2967,16 +2955,16 @@
       </c>
       <c r="E91" s="5"/>
       <c r="F91" s="11"/>
-      <c r="G91" s="16">
-        <v>1</v>
-      </c>
-      <c r="H91" s="17"/>
-      <c r="I91" s="17">
+      <c r="G91" s="14">
+        <v>1</v>
+      </c>
+      <c r="H91" s="15"/>
+      <c r="I91" s="15">
         <f t="shared" ref="I91:I103" si="13">D91-H91</f>
         <v>0.92159999999999997</v>
       </c>
-      <c r="J91" s="16"/>
-      <c r="K91" s="16"/>
+      <c r="J91" s="14"/>
+      <c r="K91" s="14"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="11"/>
@@ -2987,16 +2975,16 @@
       </c>
       <c r="E92" s="5"/>
       <c r="F92" s="11"/>
-      <c r="G92" s="16">
+      <c r="G92" s="14">
         <v>2</v>
       </c>
-      <c r="H92" s="17"/>
-      <c r="I92" s="17">
+      <c r="H92" s="15"/>
+      <c r="I92" s="15">
         <f t="shared" si="13"/>
         <v>0.92159999999999997</v>
       </c>
-      <c r="J92" s="16"/>
-      <c r="K92" s="16"/>
+      <c r="J92" s="14"/>
+      <c r="K92" s="14"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="11"/>

</xml_diff>